<commit_message>
nuevo grafico box plot
</commit_message>
<xml_diff>
--- a/datos/Base de datos.xlsx
+++ b/datos/Base de datos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e04efd92f7ba91d6/Desktop/proyecto uva de mesa/datos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e04efd92f7ba91d6/Desktop/Uva de mesa 2025/Datos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="8_{491D3EAC-A707-4E6A-A761-FD967B11B747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{729C339C-C123-42EC-8FCA-A972A2D44712}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="8_{491D3EAC-A707-4E6A-A761-FD967B11B747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0761459-AF52-4BB9-A531-8F7CED34D072}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{D9977B6E-A6B7-4838-B972-B3FE661CC160}"/>
   </bookViews>
@@ -79941,6 +79941,10 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="6" max="6" width="15.109375" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">

</xml_diff>